<commit_message>
fixes for openxlsx implementation
</commit_message>
<xml_diff>
--- a/www/Configs/NSMP/No Errors -  Entry Template - NSMP.xlsx
+++ b/www/Configs/NSMP/No Errors -  Entry Template - NSMP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/sea084_csiro_au/Documents/RossRCode/Git/Shiny/Apps/NationalSoilMonitoring/NSMData/www/Configs/NSMP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/sea084_csiro_au/Documents/RossRCode/Git/Shiny/Apps/SoilDataEntry/www/Configs/NSMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1150" documentId="13_ncr:1_{806FB16B-895D-4BC9-A51C-3E69EFC0CC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36C15B4D-C235-45DA-AE71-B54CE218DCA2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-220" windowWidth="25600" windowHeight="15500" firstSheet="1" activeTab="1" xr2:uid="{83C9EC8A-7EF8-4F9D-A138-3450D8759736}"/>
+    <workbookView xWindow="3165" yWindow="-18120" windowWidth="29040" windowHeight="18240" firstSheet="1" activeTab="7" xr2:uid="{83C9EC8A-7EF8-4F9D-A138-3450D8759736}"/>
   </bookViews>
   <sheets>
     <sheet name="TemplateOriginal" sheetId="1" state="hidden" r:id="rId1"/>
@@ -11612,7 +11612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47E6B88-97CE-436E-8F7D-17E89501757A}">
   <dimension ref="A1:AU33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
@@ -26895,7 +26895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263C6506-B5D4-4EBC-8307-876BBB7A38A3}">
   <dimension ref="A1:AU34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>

</xml_diff>